<commit_message>
EPaper-13 Account 3 Account groups and account types are separated into 2 tables.
</commit_message>
<xml_diff>
--- a/src/temp/ListChartOfAccounts.xlsx
+++ b/src/temp/ListChartOfAccounts.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24800" windowHeight="10060"/>
+    <workbookView windowWidth="25600" windowHeight="11940" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="100">
   <si>
     <t>name</t>
   </si>
@@ -276,6 +277,45 @@
   </si>
   <si>
     <t>Exchange Gain or Loss</t>
+  </si>
+  <si>
+    <t>account_type</t>
+  </si>
+  <si>
+    <t>other_current_asset</t>
+  </si>
+  <si>
+    <t>cash</t>
+  </si>
+  <si>
+    <t>fixed_asset</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>other_current_liability</t>
+  </si>
+  <si>
+    <t>long_term_liability</t>
+  </si>
+  <si>
+    <t>other_liability</t>
+  </si>
+  <si>
+    <t>equity</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>expense</t>
+  </si>
+  <si>
+    <t>cost_of_goods_sold</t>
+  </si>
+  <si>
+    <t>other_expense</t>
   </si>
 </sst>
 </file>
@@ -283,10 +323,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -297,17 +337,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <name val="timesnewroman"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="timesnewroman"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -323,18 +363,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -347,37 +395,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -391,24 +409,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -422,10 +424,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -437,14 +440,28 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -452,7 +469,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -471,6 +488,29 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -501,7 +541,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,13 +601,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,73 +661,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -621,7 +685,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -633,43 +697,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,15 +772,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -757,15 +788,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -795,153 +817,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -949,17 +989,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -1284,8 +1324,8 @@
   <sheetPr/>
   <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
@@ -1299,40 +1339,40 @@
   </cols>
   <sheetData>
     <row r="1" ht="16.8" spans="1:7">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" s="3" customFormat="1" ht="16.8" spans="1:7">
-      <c r="A2" s="5"/>
-      <c r="B2" s="3" t="s">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" s="2" customFormat="1" ht="16.8" spans="1:7">
+      <c r="A2" s="3"/>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="3">
         <v>11</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" t="s">
@@ -1414,17 +1454,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" spans="2:6">
-      <c r="B7" s="3" t="s">
+    <row r="7" s="2" customFormat="1" spans="2:6">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>12</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1468,34 +1508,34 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" s="3" customFormat="1" spans="2:7">
-      <c r="B10" s="3" t="s">
+    <row r="10" s="2" customFormat="1" spans="2:7">
+      <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>13</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>1</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" s="3" customFormat="1" spans="2:6">
-      <c r="B11" s="3" t="s">
+      <c r="G10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" s="2" customFormat="1" spans="2:6">
+      <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>14</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1519,49 +1559,49 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" s="3" customFormat="1" spans="2:6">
-      <c r="B13" s="1" t="s">
+    <row r="13" s="2" customFormat="1" spans="2:6">
+      <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="4">
         <v>15</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="3">
+      <c r="E13" s="4"/>
+      <c r="F13" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="14" s="3" customFormat="1" spans="2:6">
-      <c r="B14" s="2" t="s">
+    <row r="14" s="2" customFormat="1" spans="2:6">
+      <c r="B14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="5">
         <v>151</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F14">
         <v>15</v>
       </c>
     </row>
-    <row r="15" s="3" customFormat="1" spans="2:6">
-      <c r="B15" s="3" t="s">
+    <row r="15" s="2" customFormat="1" spans="2:6">
+      <c r="B15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>21</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1665,34 +1705,34 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" s="3" customFormat="1" spans="2:7">
-      <c r="B21" s="3" t="s">
+    <row r="21" s="2" customFormat="1" spans="2:7">
+      <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>22</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>2</v>
       </c>
-      <c r="G21" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" s="3" customFormat="1" spans="2:6">
-      <c r="B22" s="3" t="s">
+      <c r="G21" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" s="2" customFormat="1" spans="2:6">
+      <c r="B22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>23</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1736,17 +1776,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" s="3" customFormat="1" spans="2:6">
-      <c r="B25" s="3" t="s">
+    <row r="25" s="2" customFormat="1" spans="2:6">
+      <c r="B25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>24</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1770,17 +1810,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" s="3" customFormat="1" spans="2:6">
-      <c r="B27" s="3" t="s">
+    <row r="27" s="2" customFormat="1" spans="2:6">
+      <c r="B27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>31</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="2">
         <v>3</v>
       </c>
     </row>
@@ -1945,17 +1985,17 @@
       </c>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="4">
         <v>41</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="3">
+      <c r="E36" s="4"/>
+      <c r="F36" s="2">
         <v>4</v>
       </c>
       <c r="G36" t="s">
@@ -1963,16 +2003,16 @@
       </c>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="5">
         <v>411</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F37">
@@ -1983,16 +2023,16 @@
       </c>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="5">
         <v>412</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F38">
@@ -2003,16 +2043,16 @@
       </c>
     </row>
     <row r="39" spans="2:7">
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="5">
         <v>413</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F39">
@@ -2023,16 +2063,16 @@
       </c>
     </row>
     <row r="40" spans="2:7">
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="5">
         <v>414</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F40">
@@ -2043,16 +2083,16 @@
       </c>
     </row>
     <row r="41" spans="2:7">
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="5">
         <v>415</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F41">
@@ -2063,16 +2103,16 @@
       </c>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="5">
         <v>416</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E42" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F42">
@@ -2082,49 +2122,49 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" s="3" customFormat="1" spans="2:6">
-      <c r="B43" s="2" t="s">
+    <row r="43" s="2" customFormat="1" spans="2:6">
+      <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="5">
         <v>417</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E43" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F43" s="6">
         <v>41</v>
       </c>
     </row>
-    <row r="44" s="3" customFormat="1" spans="2:6">
-      <c r="B44" s="1" t="s">
+    <row r="44" s="2" customFormat="1" spans="2:6">
+      <c r="B44" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="4">
         <v>42</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="3">
+      <c r="E44" s="4"/>
+      <c r="F44" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="45" spans="2:7">
-      <c r="B45" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C45" s="1">
-        <v>51</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E45" s="1"/>
+      <c r="B45" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="4">
+        <v>51</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" s="4"/>
       <c r="F45">
         <v>5</v>
       </c>
@@ -2133,16 +2173,16 @@
       </c>
     </row>
     <row r="46" spans="2:7">
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="5">
         <v>511</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E46" s="2" t="s">
+      <c r="D46" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F46">
@@ -2153,16 +2193,16 @@
       </c>
     </row>
     <row r="47" spans="2:7">
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="5">
         <v>512</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E47" s="2" t="s">
+      <c r="D47" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F47">
@@ -2173,16 +2213,16 @@
       </c>
     </row>
     <row r="48" spans="2:7">
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="5">
         <v>513</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E48" s="2" t="s">
+      <c r="D48" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F48">
@@ -2193,16 +2233,16 @@
       </c>
     </row>
     <row r="49" spans="2:7">
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="5">
         <v>515</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E49" s="2" t="s">
+      <c r="D49" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F49">
@@ -2213,16 +2253,16 @@
       </c>
     </row>
     <row r="50" spans="2:7">
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="5">
         <v>516</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E50" s="2" t="s">
+      <c r="D50" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E50" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F50">
@@ -2233,16 +2273,16 @@
       </c>
     </row>
     <row r="51" spans="2:7">
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="5">
         <v>517</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E51" s="2" t="s">
+      <c r="D51" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E51" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F51">
@@ -2253,16 +2293,16 @@
       </c>
     </row>
     <row r="52" spans="2:7">
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="5">
         <v>518</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E52" s="2" t="s">
+      <c r="D52" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E52" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F52">
@@ -2273,16 +2313,16 @@
       </c>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="5">
         <v>519</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E53" s="2" t="s">
+      <c r="D53" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E53" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F53">
@@ -2293,16 +2333,16 @@
       </c>
     </row>
     <row r="54" spans="2:7">
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="5">
         <v>520</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E54" s="2" t="s">
+      <c r="D54" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F54">
@@ -2313,16 +2353,16 @@
       </c>
     </row>
     <row r="55" spans="2:7">
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="5">
         <v>521</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E55" s="2" t="s">
+      <c r="D55" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F55">
@@ -2333,16 +2373,16 @@
       </c>
     </row>
     <row r="56" spans="2:7">
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="5">
         <v>522</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E56" s="2" t="s">
+      <c r="D56" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E56" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F56">
@@ -2353,16 +2393,16 @@
       </c>
     </row>
     <row r="57" spans="2:7">
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="5">
         <v>523</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E57" s="2" t="s">
+      <c r="D57" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E57" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F57">
@@ -2373,16 +2413,16 @@
       </c>
     </row>
     <row r="58" spans="2:7">
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="5">
         <v>524</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E58" s="2" t="s">
+      <c r="D58" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F58">
@@ -2393,16 +2433,16 @@
       </c>
     </row>
     <row r="59" spans="2:7">
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="5">
         <v>525</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E59" s="2" t="s">
+      <c r="D59" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F59">
@@ -2413,16 +2453,16 @@
       </c>
     </row>
     <row r="60" spans="2:7">
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="5">
         <v>526</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E60" s="2" t="s">
+      <c r="D60" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F60">
@@ -2433,16 +2473,16 @@
       </c>
     </row>
     <row r="61" spans="2:7">
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="5">
         <v>527</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E61" s="2" t="s">
+      <c r="D61" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F61">
@@ -2453,16 +2493,16 @@
       </c>
     </row>
     <row r="62" spans="2:7">
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="5">
         <v>528</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E62" s="2" t="s">
+      <c r="D62" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F62">
@@ -2473,16 +2513,16 @@
       </c>
     </row>
     <row r="63" spans="2:7">
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="5">
         <v>529</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E63" s="2" t="s">
+      <c r="D63" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E63" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F63">
@@ -2493,16 +2533,16 @@
       </c>
     </row>
     <row r="64" spans="2:7">
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="5">
         <v>530</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E64" s="2" t="s">
+      <c r="D64" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E64" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F64">
@@ -2513,16 +2553,16 @@
       </c>
     </row>
     <row r="65" spans="2:7">
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="5">
         <v>531</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E65" s="2" t="s">
+      <c r="D65" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F65">
@@ -2533,16 +2573,16 @@
       </c>
     </row>
     <row r="66" spans="2:7">
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66" s="5">
         <v>532</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E66" s="2" t="s">
+      <c r="D66" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E66" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F66">
@@ -2553,16 +2593,16 @@
       </c>
     </row>
     <row r="67" spans="2:7">
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67" s="5">
         <v>533</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E67" s="2" t="s">
+      <c r="D67" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F67">
@@ -2573,16 +2613,16 @@
       </c>
     </row>
     <row r="68" spans="2:7">
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68" s="5">
         <v>534</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E68" s="2" t="s">
+      <c r="D68" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E68" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F68">
@@ -2593,16 +2633,16 @@
       </c>
     </row>
     <row r="69" spans="2:7">
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69" s="5">
         <v>535</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E69" s="2" t="s">
+      <c r="D69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E69" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F69">
@@ -2613,16 +2653,16 @@
       </c>
     </row>
     <row r="70" spans="2:7">
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70" s="5">
         <v>536</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E70" s="2" t="s">
+      <c r="D70" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E70" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F70">
@@ -2633,16 +2673,16 @@
       </c>
     </row>
     <row r="71" spans="2:7">
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71" s="5">
         <v>537</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E71" s="2" t="s">
+      <c r="D71" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F71">
@@ -2652,17 +2692,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" s="3" customFormat="1" spans="2:6">
-      <c r="B72" s="2" t="s">
+    <row r="72" s="2" customFormat="1" spans="2:6">
+      <c r="B72" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72" s="5">
         <v>538</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E72" s="2" t="s">
+      <c r="D72" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E72" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F72">
@@ -2670,17 +2710,17 @@
       </c>
     </row>
     <row r="73" spans="2:7">
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C73" s="1">
+      <c r="C73" s="4">
         <v>52</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E73" s="1"/>
-      <c r="F73" s="3">
+      <c r="D73" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E73" s="4"/>
+      <c r="F73" s="2">
         <v>5</v>
       </c>
       <c r="G73" t="s">
@@ -2688,16 +2728,16 @@
       </c>
     </row>
     <row r="74" spans="2:7">
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74" s="5">
         <v>521</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E74" s="2" t="s">
+      <c r="D74" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E74" s="5" t="s">
         <v>79</v>
       </c>
       <c r="F74">
@@ -2708,16 +2748,16 @@
       </c>
     </row>
     <row r="75" spans="2:7">
-      <c r="B75" s="2" t="s">
+      <c r="B75" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C75" s="5">
         <v>522</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E75" s="2" t="s">
+      <c r="D75" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E75" s="5" t="s">
         <v>79</v>
       </c>
       <c r="F75">
@@ -2728,16 +2768,16 @@
       </c>
     </row>
     <row r="76" spans="2:7">
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76" s="5">
         <v>523</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E76" s="2" t="s">
+      <c r="D76" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E76" s="5" t="s">
         <v>79</v>
       </c>
       <c r="F76">
@@ -2748,16 +2788,16 @@
       </c>
     </row>
     <row r="77" spans="2:7">
-      <c r="B77" s="2" t="s">
+      <c r="B77" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C77" s="5">
         <v>524</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E77" s="2" t="s">
+      <c r="D77" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E77" s="5" t="s">
         <v>79</v>
       </c>
       <c r="F77">
@@ -2768,16 +2808,16 @@
       </c>
     </row>
     <row r="78" spans="2:7">
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C78" s="2">
+      <c r="C78" s="5">
         <v>525</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E78" s="2" t="s">
+      <c r="D78" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E78" s="5" t="s">
         <v>79</v>
       </c>
       <c r="F78">
@@ -2787,32 +2827,32 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" s="3" customFormat="1" spans="2:6">
-      <c r="B79" s="1" t="s">
+    <row r="79" s="2" customFormat="1" spans="2:6">
+      <c r="B79" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C79" s="1">
+      <c r="C79" s="4">
         <v>53</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E79" s="1"/>
-      <c r="F79" s="3">
+      <c r="D79" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E79" s="4"/>
+      <c r="F79" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="80" s="3" customFormat="1" spans="2:6">
-      <c r="B80" s="2" t="s">
+    <row r="80" s="2" customFormat="1" spans="2:6">
+      <c r="B80" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C80" s="5">
         <v>526</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E80" s="2" t="s">
+      <c r="D80" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E80" s="5" t="s">
         <v>85</v>
       </c>
       <c r="F80">
@@ -2836,551 +2876,1725 @@
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D46" sqref="A1:D46"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
+      <c r="A1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F80"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="29.3125" customWidth="1"/>
+    <col min="2" max="2" width="5.625" customWidth="1"/>
+    <col min="3" max="3" width="8.3125" customWidth="1"/>
+    <col min="4" max="4" width="22.78125" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="17.8125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="16.8" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" ht="16.8" spans="1:6">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>111</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>112</v>
+      </c>
+      <c r="C4"/>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4"/>
+      <c r="F4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>113</v>
+      </c>
+      <c r="C5"/>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>114</v>
+      </c>
+      <c r="C6"/>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6"/>
+      <c r="F6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>121</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8"/>
+      <c r="F8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>122</v>
+      </c>
+      <c r="C9"/>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9"/>
+      <c r="F9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>141</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12"/>
+      <c r="F12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="5">
+        <v>151</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14"/>
+      <c r="F14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>211</v>
+      </c>
+      <c r="C16"/>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>212</v>
+      </c>
+      <c r="C17"/>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17"/>
+      <c r="F17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>213</v>
+      </c>
+      <c r="C18"/>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18"/>
+      <c r="F18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>214</v>
+      </c>
+      <c r="C19"/>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19"/>
+      <c r="F19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>215</v>
+      </c>
+      <c r="C20"/>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20"/>
+      <c r="F20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23">
+        <v>231</v>
+      </c>
+      <c r="C23"/>
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23"/>
+      <c r="F23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <v>232</v>
+      </c>
+      <c r="C24"/>
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24"/>
+      <c r="F24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26">
+        <v>241</v>
+      </c>
+      <c r="C26"/>
+      <c r="D26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26"/>
+      <c r="F26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28">
+        <v>311</v>
+      </c>
+      <c r="C28"/>
+      <c r="D28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28"/>
+      <c r="F28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29">
+        <v>312</v>
+      </c>
+      <c r="C29"/>
+      <c r="D29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29"/>
+      <c r="F29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30">
+        <v>313</v>
+      </c>
+      <c r="C30"/>
+      <c r="D30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30"/>
+      <c r="F30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31">
+        <v>314</v>
+      </c>
+      <c r="C31"/>
+      <c r="D31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31"/>
+      <c r="F31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32">
+        <v>315</v>
+      </c>
+      <c r="C32"/>
+      <c r="D32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32"/>
+      <c r="F32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33">
+        <v>316</v>
+      </c>
+      <c r="C33"/>
+      <c r="D33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33"/>
+      <c r="F33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34">
+        <v>317</v>
+      </c>
+      <c r="C34"/>
+      <c r="D34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34"/>
+      <c r="F34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35">
+        <v>318</v>
+      </c>
+      <c r="C35"/>
+      <c r="D35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35"/>
+      <c r="F35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="5">
+        <v>411</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="E37"/>
+      <c r="F37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="5">
+        <v>412</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
+      <c r="E38"/>
+      <c r="F38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="5">
+        <v>413</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E39"/>
+      <c r="F39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="5">
+        <v>414</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="E40"/>
+      <c r="F40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="5">
+        <v>415</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E41"/>
+      <c r="F41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="5">
+        <v>416</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
+      <c r="E42"/>
+      <c r="F42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="5">
+        <v>417</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="2" t="s">
+      <c r="E43" s="6"/>
+      <c r="F43" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="2" t="s">
+      <c r="B46" s="5">
+        <v>511</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46"/>
+      <c r="F46" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="2" t="s">
+      <c r="B47" s="5">
+        <v>512</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47"/>
+      <c r="F47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="2" t="s">
+      <c r="B48" s="5">
+        <v>513</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48"/>
+      <c r="F48" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
+      <c r="B49" s="5">
+        <v>515</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E49"/>
+      <c r="F49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="2" t="s">
+      <c r="B50" s="5">
+        <v>516</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E50"/>
+      <c r="F50" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="2" t="s">
+      <c r="B51" s="5">
+        <v>517</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E51"/>
+      <c r="F51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="2" t="s">
+      <c r="B52" s="5">
+        <v>518</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E52"/>
+      <c r="F52" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="2" t="s">
+      <c r="B53" s="5">
+        <v>519</v>
+      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E53"/>
+      <c r="F53" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="2" t="s">
+      <c r="B54" s="5">
+        <v>520</v>
+      </c>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E54"/>
+      <c r="F54" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="2" t="s">
+      <c r="B55" s="5">
+        <v>521</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E55"/>
+      <c r="F55" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="2" t="s">
+      <c r="B56" s="5">
+        <v>522</v>
+      </c>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E56"/>
+      <c r="F56" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="2" t="s">
+      <c r="B57" s="5">
+        <v>523</v>
+      </c>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E57"/>
+      <c r="F57" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="2" t="s">
+      <c r="B58" s="5">
+        <v>524</v>
+      </c>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E58"/>
+      <c r="F58" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="2" t="s">
+      <c r="B59" s="5">
+        <v>525</v>
+      </c>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E59"/>
+      <c r="F59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="2" t="s">
+      <c r="B60" s="5">
+        <v>526</v>
+      </c>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E60"/>
+      <c r="F60" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="2" t="s">
+      <c r="B61" s="5">
+        <v>527</v>
+      </c>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E61"/>
+      <c r="F61" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="2" t="s">
+      <c r="B62" s="5">
+        <v>528</v>
+      </c>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E62"/>
+      <c r="F62" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="2" t="s">
+      <c r="B63" s="5">
+        <v>529</v>
+      </c>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E63"/>
+      <c r="F63" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="2" t="s">
+      <c r="B64" s="5">
+        <v>530</v>
+      </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E64"/>
+      <c r="F64" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="2" t="s">
+      <c r="B65" s="5">
+        <v>531</v>
+      </c>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E65"/>
+      <c r="F65" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="2" t="s">
+      <c r="B66" s="5">
+        <v>532</v>
+      </c>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E66"/>
+      <c r="F66" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="2" t="s">
+      <c r="B67" s="5">
+        <v>533</v>
+      </c>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E67"/>
+      <c r="F67" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="2" t="s">
+      <c r="B68" s="5">
+        <v>534</v>
+      </c>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E68"/>
+      <c r="F68" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="2" t="s">
+      <c r="B69" s="5">
+        <v>535</v>
+      </c>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E69"/>
+      <c r="F69" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="2" t="s">
+      <c r="B70" s="5">
+        <v>536</v>
+      </c>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E70"/>
+      <c r="F70" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="2" t="s">
+      <c r="B71" s="5">
+        <v>537</v>
+      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E71"/>
+      <c r="F71" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="1" t="s">
+      <c r="B72" s="5">
+        <v>538</v>
+      </c>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E72"/>
+      <c r="F72" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="2"/>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B74" s="5">
+        <v>521</v>
+      </c>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="E74"/>
+      <c r="F74" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B75" s="5">
+        <v>522</v>
+      </c>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="E75"/>
+      <c r="F75" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B76" s="5">
+        <v>523</v>
+      </c>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="E76"/>
+      <c r="F76" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B77" s="5">
+        <v>524</v>
+      </c>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="E77"/>
+      <c r="F77" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B78" s="5">
+        <v>525</v>
+      </c>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="2" t="s">
+      <c r="E78"/>
+      <c r="F78" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="2"/>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="B80" s="5">
+        <v>526</v>
+      </c>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="1"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>18</v>
+      <c r="E80"/>
+      <c r="F80" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
account template data import fixed.
</commit_message>
<xml_diff>
--- a/src/temp/ListChartOfAccounts.xlsx
+++ b/src/temp/ListChartOfAccounts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="11940" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="104">
   <si>
     <t>name</t>
   </si>
@@ -316,6 +316,18 @@
   </si>
   <si>
     <t>other_expense</t>
+  </si>
+  <si>
+    <t>Input Tax</t>
+  </si>
+  <si>
+    <t>input_tax</t>
+  </si>
+  <si>
+    <t>Output Tax</t>
+  </si>
+  <si>
+    <t>output_tax</t>
   </si>
 </sst>
 </file>
@@ -323,10 +335,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -364,7 +376,74 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -378,98 +457,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -492,17 +481,33 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -511,6 +516,13 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -541,7 +553,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -553,13 +595,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -571,49 +607,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -631,25 +625,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -661,7 +661,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -673,7 +685,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,31 +703,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -753,6 +765,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -768,15 +798,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -788,6 +809,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -817,171 +847,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1324,7 +1336,7 @@
   <sheetPr/>
   <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:F80"/>
     </sheetView>
   </sheetViews>
@@ -2875,7 +2887,7 @@
   <sheetPr/>
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A78" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -3432,10 +3444,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="H87" sqref="H87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3483,11 +3495,9 @@
       <c r="B3">
         <v>111</v>
       </c>
-      <c r="C3"/>
       <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="E3"/>
       <c r="F3" t="s">
         <v>88</v>
       </c>
@@ -3499,11 +3509,9 @@
       <c r="B4">
         <v>112</v>
       </c>
-      <c r="C4"/>
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E4"/>
       <c r="F4" t="s">
         <v>88</v>
       </c>
@@ -3515,11 +3523,9 @@
       <c r="B5">
         <v>113</v>
       </c>
-      <c r="C5"/>
       <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="E5"/>
       <c r="F5" t="s">
         <v>88</v>
       </c>
@@ -3531,11 +3537,9 @@
       <c r="B6">
         <v>114</v>
       </c>
-      <c r="C6"/>
       <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="E6"/>
       <c r="F6" t="s">
         <v>88</v>
       </c>
@@ -3554,11 +3558,9 @@
       <c r="B8">
         <v>121</v>
       </c>
-      <c r="C8"/>
       <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="E8"/>
       <c r="F8" t="s">
         <v>89</v>
       </c>
@@ -3570,11 +3572,9 @@
       <c r="B9">
         <v>122</v>
       </c>
-      <c r="C9"/>
       <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="E9"/>
       <c r="F9" t="s">
         <v>89</v>
       </c>
@@ -3600,11 +3600,9 @@
       <c r="B12">
         <v>141</v>
       </c>
-      <c r="C12"/>
       <c r="D12" t="s">
         <v>16</v>
       </c>
-      <c r="E12"/>
       <c r="F12" t="s">
         <v>90</v>
       </c>
@@ -3627,7 +3625,6 @@
       <c r="D14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E14"/>
       <c r="F14" t="s">
         <v>91</v>
       </c>
@@ -3646,11 +3643,9 @@
       <c r="B16">
         <v>211</v>
       </c>
-      <c r="C16"/>
       <c r="D16" t="s">
         <v>20</v>
       </c>
-      <c r="E16"/>
       <c r="F16" t="s">
         <v>92</v>
       </c>
@@ -3662,11 +3657,9 @@
       <c r="B17">
         <v>212</v>
       </c>
-      <c r="C17"/>
       <c r="D17" t="s">
         <v>20</v>
       </c>
-      <c r="E17"/>
       <c r="F17" t="s">
         <v>92</v>
       </c>
@@ -3678,11 +3671,9 @@
       <c r="B18">
         <v>213</v>
       </c>
-      <c r="C18"/>
       <c r="D18" t="s">
         <v>20</v>
       </c>
-      <c r="E18"/>
       <c r="F18" t="s">
         <v>92</v>
       </c>
@@ -3694,11 +3685,9 @@
       <c r="B19">
         <v>214</v>
       </c>
-      <c r="C19"/>
       <c r="D19" t="s">
         <v>20</v>
       </c>
-      <c r="E19"/>
       <c r="F19" t="s">
         <v>92</v>
       </c>
@@ -3710,11 +3699,9 @@
       <c r="B20">
         <v>215</v>
       </c>
-      <c r="C20"/>
       <c r="D20" t="s">
         <v>20</v>
       </c>
-      <c r="E20"/>
       <c r="F20" t="s">
         <v>92</v>
       </c>
@@ -3740,11 +3727,9 @@
       <c r="B23">
         <v>231</v>
       </c>
-      <c r="C23"/>
       <c r="D23" t="s">
         <v>28</v>
       </c>
-      <c r="E23"/>
       <c r="F23" t="s">
         <v>93</v>
       </c>
@@ -3756,11 +3741,9 @@
       <c r="B24">
         <v>232</v>
       </c>
-      <c r="C24"/>
       <c r="D24" t="s">
         <v>28</v>
       </c>
-      <c r="E24"/>
       <c r="F24" t="s">
         <v>93</v>
       </c>
@@ -3779,11 +3762,9 @@
       <c r="B26">
         <v>241</v>
       </c>
-      <c r="C26"/>
       <c r="D26" t="s">
         <v>31</v>
       </c>
-      <c r="E26"/>
       <c r="F26" t="s">
         <v>94</v>
       </c>
@@ -3802,11 +3783,9 @@
       <c r="B28">
         <v>311</v>
       </c>
-      <c r="C28"/>
       <c r="D28" t="s">
         <v>33</v>
       </c>
-      <c r="E28"/>
       <c r="F28" t="s">
         <v>95</v>
       </c>
@@ -3818,11 +3797,9 @@
       <c r="B29">
         <v>312</v>
       </c>
-      <c r="C29"/>
       <c r="D29" t="s">
         <v>33</v>
       </c>
-      <c r="E29"/>
       <c r="F29" t="s">
         <v>95</v>
       </c>
@@ -3834,11 +3811,9 @@
       <c r="B30">
         <v>313</v>
       </c>
-      <c r="C30"/>
       <c r="D30" t="s">
         <v>33</v>
       </c>
-      <c r="E30"/>
       <c r="F30" t="s">
         <v>95</v>
       </c>
@@ -3850,11 +3825,9 @@
       <c r="B31">
         <v>314</v>
       </c>
-      <c r="C31"/>
       <c r="D31" t="s">
         <v>33</v>
       </c>
-      <c r="E31"/>
       <c r="F31" t="s">
         <v>95</v>
       </c>
@@ -3866,11 +3839,9 @@
       <c r="B32">
         <v>315</v>
       </c>
-      <c r="C32"/>
       <c r="D32" t="s">
         <v>33</v>
       </c>
-      <c r="E32"/>
       <c r="F32" t="s">
         <v>95</v>
       </c>
@@ -3882,11 +3853,9 @@
       <c r="B33">
         <v>316</v>
       </c>
-      <c r="C33"/>
       <c r="D33" t="s">
         <v>33</v>
       </c>
-      <c r="E33"/>
       <c r="F33" t="s">
         <v>95</v>
       </c>
@@ -3898,11 +3867,9 @@
       <c r="B34">
         <v>317</v>
       </c>
-      <c r="C34"/>
       <c r="D34" t="s">
         <v>33</v>
       </c>
-      <c r="E34"/>
       <c r="F34" t="s">
         <v>95</v>
       </c>
@@ -3914,11 +3881,9 @@
       <c r="B35">
         <v>318</v>
       </c>
-      <c r="C35"/>
       <c r="D35" t="s">
         <v>33</v>
       </c>
-      <c r="E35"/>
       <c r="F35" t="s">
         <v>95</v>
       </c>
@@ -3941,7 +3906,6 @@
       <c r="D37" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E37"/>
       <c r="F37" t="s">
         <v>96</v>
       </c>
@@ -3957,7 +3921,6 @@
       <c r="D38" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E38"/>
       <c r="F38" t="s">
         <v>96</v>
       </c>
@@ -3973,7 +3936,6 @@
       <c r="D39" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E39"/>
       <c r="F39" t="s">
         <v>96</v>
       </c>
@@ -3989,7 +3951,6 @@
       <c r="D40" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E40"/>
       <c r="F40" t="s">
         <v>96</v>
       </c>
@@ -4005,7 +3966,6 @@
       <c r="D41" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E41"/>
       <c r="F41" t="s">
         <v>96</v>
       </c>
@@ -4021,7 +3981,6 @@
       <c r="D42" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E42"/>
       <c r="F42" t="s">
         <v>96</v>
       </c>
@@ -4066,7 +4025,6 @@
       <c r="D46" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E46"/>
       <c r="F46" t="s">
         <v>97</v>
       </c>
@@ -4082,7 +4040,6 @@
       <c r="D47" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E47"/>
       <c r="F47" t="s">
         <v>97</v>
       </c>
@@ -4098,7 +4055,6 @@
       <c r="D48" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E48"/>
       <c r="F48" t="s">
         <v>97</v>
       </c>
@@ -4114,7 +4070,6 @@
       <c r="D49" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E49"/>
       <c r="F49" t="s">
         <v>97</v>
       </c>
@@ -4130,7 +4085,6 @@
       <c r="D50" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E50"/>
       <c r="F50" t="s">
         <v>97</v>
       </c>
@@ -4146,7 +4100,6 @@
       <c r="D51" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E51"/>
       <c r="F51" t="s">
         <v>97</v>
       </c>
@@ -4162,7 +4115,6 @@
       <c r="D52" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E52"/>
       <c r="F52" t="s">
         <v>97</v>
       </c>
@@ -4178,7 +4130,6 @@
       <c r="D53" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E53"/>
       <c r="F53" t="s">
         <v>97</v>
       </c>
@@ -4194,7 +4145,6 @@
       <c r="D54" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E54"/>
       <c r="F54" t="s">
         <v>97</v>
       </c>
@@ -4210,7 +4160,6 @@
       <c r="D55" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E55"/>
       <c r="F55" t="s">
         <v>97</v>
       </c>
@@ -4226,7 +4175,6 @@
       <c r="D56" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E56"/>
       <c r="F56" t="s">
         <v>97</v>
       </c>
@@ -4242,7 +4190,6 @@
       <c r="D57" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E57"/>
       <c r="F57" t="s">
         <v>97</v>
       </c>
@@ -4258,7 +4205,6 @@
       <c r="D58" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E58"/>
       <c r="F58" t="s">
         <v>97</v>
       </c>
@@ -4274,7 +4220,6 @@
       <c r="D59" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E59"/>
       <c r="F59" t="s">
         <v>97</v>
       </c>
@@ -4290,7 +4235,6 @@
       <c r="D60" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E60"/>
       <c r="F60" t="s">
         <v>97</v>
       </c>
@@ -4306,7 +4250,6 @@
       <c r="D61" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E61"/>
       <c r="F61" t="s">
         <v>97</v>
       </c>
@@ -4322,7 +4265,6 @@
       <c r="D62" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E62"/>
       <c r="F62" t="s">
         <v>97</v>
       </c>
@@ -4338,7 +4280,6 @@
       <c r="D63" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E63"/>
       <c r="F63" t="s">
         <v>97</v>
       </c>
@@ -4354,7 +4295,6 @@
       <c r="D64" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E64"/>
       <c r="F64" t="s">
         <v>97</v>
       </c>
@@ -4370,7 +4310,6 @@
       <c r="D65" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E65"/>
       <c r="F65" t="s">
         <v>97</v>
       </c>
@@ -4386,7 +4325,6 @@
       <c r="D66" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E66"/>
       <c r="F66" t="s">
         <v>97</v>
       </c>
@@ -4402,7 +4340,6 @@
       <c r="D67" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E67"/>
       <c r="F67" t="s">
         <v>97</v>
       </c>
@@ -4418,7 +4355,6 @@
       <c r="D68" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E68"/>
       <c r="F68" t="s">
         <v>97</v>
       </c>
@@ -4434,7 +4370,6 @@
       <c r="D69" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E69"/>
       <c r="F69" t="s">
         <v>97</v>
       </c>
@@ -4450,7 +4385,6 @@
       <c r="D70" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E70"/>
       <c r="F70" t="s">
         <v>97</v>
       </c>
@@ -4466,7 +4400,6 @@
       <c r="D71" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E71"/>
       <c r="F71" t="s">
         <v>97</v>
       </c>
@@ -4482,7 +4415,6 @@
       <c r="D72" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E72"/>
       <c r="F72" t="s">
         <v>97</v>
       </c>
@@ -4505,7 +4437,6 @@
       <c r="D74" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E74"/>
       <c r="F74" t="s">
         <v>98</v>
       </c>
@@ -4521,7 +4452,6 @@
       <c r="D75" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E75"/>
       <c r="F75" t="s">
         <v>98</v>
       </c>
@@ -4537,7 +4467,6 @@
       <c r="D76" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E76"/>
       <c r="F76" t="s">
         <v>98</v>
       </c>
@@ -4553,7 +4482,6 @@
       <c r="D77" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E77"/>
       <c r="F77" t="s">
         <v>98</v>
       </c>
@@ -4569,7 +4497,6 @@
       <c r="D78" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E78"/>
       <c r="F78" t="s">
         <v>98</v>
       </c>
@@ -4592,9 +4519,36 @@
       <c r="D80" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E80"/>
       <c r="F80" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" t="s">
+        <v>100</v>
+      </c>
+      <c r="B82">
+        <v>161</v>
+      </c>
+      <c r="D82" t="s">
+        <v>100</v>
+      </c>
+      <c r="F82" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" t="s">
+        <v>102</v>
+      </c>
+      <c r="B83">
+        <v>251</v>
+      </c>
+      <c r="D83" t="s">
+        <v>102</v>
+      </c>
+      <c r="F83" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>